<commit_message>
Moved Directory of TAG RG to Raw Subfolder
</commit_message>
<xml_diff>
--- a/Cleaned_Tagoloan/Duplicated Values.xlsx
+++ b/Cleaned_Tagoloan/Duplicated Values.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6304" uniqueCount="2651">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6334" uniqueCount="2666">
   <si>
     <t>Water_Level</t>
   </si>
@@ -7969,6 +7969,51 @@
   </si>
   <si>
     <t>2021/09/03 09:00:00</t>
+  </si>
+  <si>
+    <t>2022/01/01 00:00:00</t>
+  </si>
+  <si>
+    <t>2022/01/01 01:00:00</t>
+  </si>
+  <si>
+    <t>2022/01/01 02:00:00</t>
+  </si>
+  <si>
+    <t>2022/01/01 03:00:00</t>
+  </si>
+  <si>
+    <t>2022/01/01 04:00:00</t>
+  </si>
+  <si>
+    <t>2022/01/01 05:00:00</t>
+  </si>
+  <si>
+    <t>2022/01/01 06:00:00</t>
+  </si>
+  <si>
+    <t>2022/01/01 07:00:00</t>
+  </si>
+  <si>
+    <t>2022/01/01 08:00:00</t>
+  </si>
+  <si>
+    <t>2022/01/01 09:00:00</t>
+  </si>
+  <si>
+    <t>2022/01/01 10:00:00</t>
+  </si>
+  <si>
+    <t>2022/01/01 11:00:00</t>
+  </si>
+  <si>
+    <t>2022/01/01 12:00:00</t>
+  </si>
+  <si>
+    <t>2022/01/01 13:00:00</t>
+  </si>
+  <si>
+    <t>2022/01/01 14:00:00</t>
   </si>
 </sst>
 </file>
@@ -15833,7 +15878,7 @@
         <v>465</v>
       </c>
       <c r="B938">
-        <v>0.9863149999999988</v>
+        <v>0.9863149999999991</v>
       </c>
     </row>
     <row r="939" spans="1:2">
@@ -15841,7 +15886,7 @@
         <v>465</v>
       </c>
       <c r="B939">
-        <v>0.9863149999999988</v>
+        <v>0.9863149999999991</v>
       </c>
     </row>
     <row r="940" spans="1:2">
@@ -15849,7 +15894,7 @@
         <v>466</v>
       </c>
       <c r="B940">
-        <v>0.5804399999999991</v>
+        <v>0.580439999999999</v>
       </c>
     </row>
     <row r="941" spans="1:2">
@@ -15857,7 +15902,7 @@
         <v>466</v>
       </c>
       <c r="B941">
-        <v>0.5804399999999991</v>
+        <v>0.580439999999999</v>
       </c>
     </row>
     <row r="942" spans="1:2">
@@ -15865,7 +15910,7 @@
         <v>467</v>
       </c>
       <c r="B942">
-        <v>0.4610649999999999</v>
+        <v>0.461065</v>
       </c>
     </row>
     <row r="943" spans="1:2">
@@ -15873,7 +15918,7 @@
         <v>467</v>
       </c>
       <c r="B943">
-        <v>0.4610649999999999</v>
+        <v>0.461065</v>
       </c>
     </row>
     <row r="944" spans="1:2">
@@ -15881,7 +15926,7 @@
         <v>468</v>
       </c>
       <c r="B944">
-        <v>0.9863149999999988</v>
+        <v>0.9863149999999991</v>
       </c>
     </row>
     <row r="945" spans="1:2">
@@ -15889,7 +15934,7 @@
         <v>468</v>
       </c>
       <c r="B945">
-        <v>0.9863149999999988</v>
+        <v>0.9863149999999991</v>
       </c>
     </row>
     <row r="946" spans="1:2">
@@ -15897,7 +15942,7 @@
         <v>469</v>
       </c>
       <c r="B946">
-        <v>0.9863149999999988</v>
+        <v>0.9863149999999991</v>
       </c>
     </row>
     <row r="947" spans="1:2">
@@ -15905,7 +15950,7 @@
         <v>469</v>
       </c>
       <c r="B947">
-        <v>0.9863149999999988</v>
+        <v>0.9863149999999991</v>
       </c>
     </row>
     <row r="948" spans="1:2">
@@ -15913,7 +15958,7 @@
         <v>470</v>
       </c>
       <c r="B948">
-        <v>0.8669399999999999</v>
+        <v>0.86694</v>
       </c>
     </row>
     <row r="949" spans="1:2">
@@ -15921,7 +15966,7 @@
         <v>470</v>
       </c>
       <c r="B949">
-        <v>0.8669399999999999</v>
+        <v>0.86694</v>
       </c>
     </row>
     <row r="950" spans="1:2">
@@ -19088,7 +19133,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B4959"/>
+  <dimension ref="A1:B4989"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -20723,7 +20768,7 @@
         <v>125</v>
       </c>
       <c r="B204">
-        <v>0.1119999999999999</v>
+        <v>0.112</v>
       </c>
     </row>
     <row r="205" spans="1:2">
@@ -20731,7 +20776,7 @@
         <v>125</v>
       </c>
       <c r="B205">
-        <v>0.1119999999999999</v>
+        <v>0.112</v>
       </c>
     </row>
     <row r="206" spans="1:2">
@@ -20739,7 +20784,7 @@
         <v>125</v>
       </c>
       <c r="B206">
-        <v>0.1119999999999999</v>
+        <v>0.112</v>
       </c>
     </row>
     <row r="207" spans="1:2">
@@ -20747,7 +20792,7 @@
         <v>126</v>
       </c>
       <c r="B207">
-        <v>0.1119999999999999</v>
+        <v>0.112</v>
       </c>
     </row>
     <row r="208" spans="1:2">
@@ -20755,7 +20800,7 @@
         <v>126</v>
       </c>
       <c r="B208">
-        <v>0.1119999999999999</v>
+        <v>0.112</v>
       </c>
     </row>
     <row r="209" spans="1:2">
@@ -20763,7 +20808,7 @@
         <v>126</v>
       </c>
       <c r="B209">
-        <v>0.1119999999999999</v>
+        <v>0.112</v>
       </c>
     </row>
     <row r="210" spans="1:2">
@@ -20771,7 +20816,7 @@
         <v>127</v>
       </c>
       <c r="B210">
-        <v>0.1119999999999999</v>
+        <v>0.112</v>
       </c>
     </row>
     <row r="211" spans="1:2">
@@ -20779,7 +20824,7 @@
         <v>127</v>
       </c>
       <c r="B211">
-        <v>0.1119999999999999</v>
+        <v>0.112</v>
       </c>
     </row>
     <row r="212" spans="1:2">
@@ -20787,7 +20832,7 @@
         <v>127</v>
       </c>
       <c r="B212">
-        <v>0.1119999999999999</v>
+        <v>0.112</v>
       </c>
     </row>
     <row r="213" spans="1:2">
@@ -20795,7 +20840,7 @@
         <v>128</v>
       </c>
       <c r="B213">
-        <v>0.1119999999999999</v>
+        <v>0.112</v>
       </c>
     </row>
     <row r="214" spans="1:2">
@@ -20803,7 +20848,7 @@
         <v>128</v>
       </c>
       <c r="B214">
-        <v>0.1119999999999999</v>
+        <v>0.112</v>
       </c>
     </row>
     <row r="215" spans="1:2">
@@ -20811,7 +20856,7 @@
         <v>128</v>
       </c>
       <c r="B215">
-        <v>0.1119999999999999</v>
+        <v>0.112</v>
       </c>
     </row>
     <row r="216" spans="1:2">
@@ -20819,7 +20864,7 @@
         <v>129</v>
       </c>
       <c r="B216">
-        <v>0.1119999999999999</v>
+        <v>0.112</v>
       </c>
     </row>
     <row r="217" spans="1:2">
@@ -20827,7 +20872,7 @@
         <v>129</v>
       </c>
       <c r="B217">
-        <v>0.1119999999999999</v>
+        <v>0.112</v>
       </c>
     </row>
     <row r="218" spans="1:2">
@@ -20835,7 +20880,7 @@
         <v>129</v>
       </c>
       <c r="B218">
-        <v>0.1119999999999999</v>
+        <v>0.112</v>
       </c>
     </row>
     <row r="219" spans="1:2">
@@ -20843,7 +20888,7 @@
         <v>130</v>
       </c>
       <c r="B219">
-        <v>0.1119999999999999</v>
+        <v>0.112</v>
       </c>
     </row>
     <row r="220" spans="1:2">
@@ -20851,7 +20896,7 @@
         <v>130</v>
       </c>
       <c r="B220">
-        <v>0.1119999999999999</v>
+        <v>0.112</v>
       </c>
     </row>
     <row r="221" spans="1:2">
@@ -20859,7 +20904,7 @@
         <v>130</v>
       </c>
       <c r="B221">
-        <v>0.1119999999999999</v>
+        <v>0.112</v>
       </c>
     </row>
     <row r="222" spans="1:2">
@@ -20867,7 +20912,7 @@
         <v>131</v>
       </c>
       <c r="B222">
-        <v>0.1119999999999999</v>
+        <v>0.112</v>
       </c>
     </row>
     <row r="223" spans="1:2">
@@ -20875,7 +20920,7 @@
         <v>131</v>
       </c>
       <c r="B223">
-        <v>0.1119999999999999</v>
+        <v>0.112</v>
       </c>
     </row>
     <row r="224" spans="1:2">
@@ -20883,7 +20928,7 @@
         <v>131</v>
       </c>
       <c r="B224">
-        <v>0.1119999999999999</v>
+        <v>0.112</v>
       </c>
     </row>
     <row r="225" spans="1:2">
@@ -20891,7 +20936,7 @@
         <v>132</v>
       </c>
       <c r="B225">
-        <v>0.1119999999999999</v>
+        <v>0.112</v>
       </c>
     </row>
     <row r="226" spans="1:2">
@@ -20899,7 +20944,7 @@
         <v>132</v>
       </c>
       <c r="B226">
-        <v>0.1119999999999999</v>
+        <v>0.112</v>
       </c>
     </row>
     <row r="227" spans="1:2">
@@ -20907,7 +20952,7 @@
         <v>132</v>
       </c>
       <c r="B227">
-        <v>0.1119999999999999</v>
+        <v>0.112</v>
       </c>
     </row>
     <row r="228" spans="1:2">
@@ -20915,7 +20960,7 @@
         <v>133</v>
       </c>
       <c r="B228">
-        <v>0.1119999999999999</v>
+        <v>0.112</v>
       </c>
     </row>
     <row r="229" spans="1:2">
@@ -20923,7 +20968,7 @@
         <v>133</v>
       </c>
       <c r="B229">
-        <v>0.1119999999999999</v>
+        <v>0.112</v>
       </c>
     </row>
     <row r="230" spans="1:2">
@@ -20931,7 +20976,7 @@
         <v>133</v>
       </c>
       <c r="B230">
-        <v>0.1119999999999999</v>
+        <v>0.112</v>
       </c>
     </row>
     <row r="231" spans="1:2">
@@ -20939,7 +20984,7 @@
         <v>134</v>
       </c>
       <c r="B231">
-        <v>0.1119999999999999</v>
+        <v>0.112</v>
       </c>
     </row>
     <row r="232" spans="1:2">
@@ -20947,7 +20992,7 @@
         <v>134</v>
       </c>
       <c r="B232">
-        <v>0.1119999999999999</v>
+        <v>0.112</v>
       </c>
     </row>
     <row r="233" spans="1:2">
@@ -20955,7 +21000,7 @@
         <v>134</v>
       </c>
       <c r="B233">
-        <v>0.1119999999999999</v>
+        <v>0.112</v>
       </c>
     </row>
     <row r="234" spans="1:2">
@@ -20963,7 +21008,7 @@
         <v>135</v>
       </c>
       <c r="B234">
-        <v>0.1119999999999999</v>
+        <v>0.112</v>
       </c>
     </row>
     <row r="235" spans="1:2">
@@ -20971,7 +21016,7 @@
         <v>135</v>
       </c>
       <c r="B235">
-        <v>0.1119999999999999</v>
+        <v>0.112</v>
       </c>
     </row>
     <row r="236" spans="1:2">
@@ -20979,7 +21024,7 @@
         <v>135</v>
       </c>
       <c r="B236">
-        <v>0.1119999999999999</v>
+        <v>0.112</v>
       </c>
     </row>
     <row r="237" spans="1:2">
@@ -20987,7 +21032,7 @@
         <v>136</v>
       </c>
       <c r="B237">
-        <v>0.1119999999999999</v>
+        <v>0.112</v>
       </c>
     </row>
     <row r="238" spans="1:2">
@@ -20995,7 +21040,7 @@
         <v>136</v>
       </c>
       <c r="B238">
-        <v>0.1119999999999999</v>
+        <v>0.112</v>
       </c>
     </row>
     <row r="239" spans="1:2">
@@ -21003,7 +21048,7 @@
         <v>136</v>
       </c>
       <c r="B239">
-        <v>0.1119999999999999</v>
+        <v>0.112</v>
       </c>
     </row>
     <row r="240" spans="1:2">
@@ -21011,7 +21056,7 @@
         <v>137</v>
       </c>
       <c r="B240">
-        <v>0.1119999999999999</v>
+        <v>0.112</v>
       </c>
     </row>
     <row r="241" spans="1:2">
@@ -21019,7 +21064,7 @@
         <v>137</v>
       </c>
       <c r="B241">
-        <v>0.1119999999999999</v>
+        <v>0.112</v>
       </c>
     </row>
     <row r="242" spans="1:2">
@@ -21027,7 +21072,7 @@
         <v>137</v>
       </c>
       <c r="B242">
-        <v>0.1119999999999999</v>
+        <v>0.112</v>
       </c>
     </row>
     <row r="243" spans="1:2">
@@ -21035,7 +21080,7 @@
         <v>138</v>
       </c>
       <c r="B243">
-        <v>0.1119999999999999</v>
+        <v>0.112</v>
       </c>
     </row>
     <row r="244" spans="1:2">
@@ -21043,7 +21088,7 @@
         <v>138</v>
       </c>
       <c r="B244">
-        <v>0.1119999999999999</v>
+        <v>0.112</v>
       </c>
     </row>
     <row r="245" spans="1:2">
@@ -21051,7 +21096,7 @@
         <v>138</v>
       </c>
       <c r="B245">
-        <v>0.1119999999999999</v>
+        <v>0.112</v>
       </c>
     </row>
     <row r="246" spans="1:2">
@@ -21171,7 +21216,7 @@
         <v>495</v>
       </c>
       <c r="B260">
-        <v>0.7120000000000001</v>
+        <v>0.712</v>
       </c>
     </row>
     <row r="261" spans="1:2">
@@ -21179,7 +21224,7 @@
         <v>495</v>
       </c>
       <c r="B261">
-        <v>0.7120000000000001</v>
+        <v>0.712</v>
       </c>
     </row>
     <row r="262" spans="1:2">
@@ -21187,7 +21232,7 @@
         <v>496</v>
       </c>
       <c r="B262">
-        <v>0.7120000000000001</v>
+        <v>0.712</v>
       </c>
     </row>
     <row r="263" spans="1:2">
@@ -21195,7 +21240,7 @@
         <v>496</v>
       </c>
       <c r="B263">
-        <v>0.7120000000000001</v>
+        <v>0.712</v>
       </c>
     </row>
     <row r="264" spans="1:2">
@@ -21203,7 +21248,7 @@
         <v>497</v>
       </c>
       <c r="B264">
-        <v>0.7120000000000001</v>
+        <v>0.712</v>
       </c>
     </row>
     <row r="265" spans="1:2">
@@ -21211,7 +21256,7 @@
         <v>497</v>
       </c>
       <c r="B265">
-        <v>0.7120000000000001</v>
+        <v>0.712</v>
       </c>
     </row>
     <row r="266" spans="1:2">
@@ -23299,7 +23344,7 @@
         <v>628</v>
       </c>
       <c r="B526">
-        <v>0.4479999999999999</v>
+        <v>0.448</v>
       </c>
     </row>
     <row r="527" spans="1:2">
@@ -23307,7 +23352,7 @@
         <v>628</v>
       </c>
       <c r="B527">
-        <v>0.4479999999999999</v>
+        <v>0.448</v>
       </c>
     </row>
     <row r="528" spans="1:2">
@@ -26067,7 +26112,7 @@
         <v>801</v>
       </c>
       <c r="B872">
-        <v>0.5920000000000001</v>
+        <v>0.592</v>
       </c>
     </row>
     <row r="873" spans="1:2">
@@ -26075,7 +26120,7 @@
         <v>801</v>
       </c>
       <c r="B873">
-        <v>0.5920000000000001</v>
+        <v>0.592</v>
       </c>
     </row>
     <row r="874" spans="1:2">
@@ -28339,7 +28384,7 @@
         <v>943</v>
       </c>
       <c r="B1156">
-        <v>0.4639999999999999</v>
+        <v>0.464</v>
       </c>
     </row>
     <row r="1157" spans="1:2">
@@ -28347,7 +28392,7 @@
         <v>943</v>
       </c>
       <c r="B1157">
-        <v>0.4639999999999999</v>
+        <v>0.464</v>
       </c>
     </row>
     <row r="1158" spans="1:2">
@@ -31091,7 +31136,7 @@
         <v>1115</v>
       </c>
       <c r="B1500">
-        <v>0.8959999999999999</v>
+        <v>0.896</v>
       </c>
     </row>
     <row r="1501" spans="1:2">
@@ -31099,7 +31144,7 @@
         <v>1115</v>
       </c>
       <c r="B1501">
-        <v>0.8959999999999999</v>
+        <v>0.896</v>
       </c>
     </row>
     <row r="1502" spans="1:2">
@@ -31603,7 +31648,7 @@
         <v>1147</v>
       </c>
       <c r="B1564">
-        <v>0.4479999999999999</v>
+        <v>0.448</v>
       </c>
     </row>
     <row r="1565" spans="1:2">
@@ -31611,7 +31656,7 @@
         <v>1147</v>
       </c>
       <c r="B1565">
-        <v>0.4479999999999999</v>
+        <v>0.448</v>
       </c>
     </row>
     <row r="1566" spans="1:2">
@@ -31619,7 +31664,7 @@
         <v>1148</v>
       </c>
       <c r="B1566">
-        <v>0.4479999999999999</v>
+        <v>0.448</v>
       </c>
     </row>
     <row r="1567" spans="1:2">
@@ -31627,7 +31672,7 @@
         <v>1148</v>
       </c>
       <c r="B1567">
-        <v>0.4479999999999999</v>
+        <v>0.448</v>
       </c>
     </row>
     <row r="1568" spans="1:2">
@@ -32435,7 +32480,7 @@
         <v>1199</v>
       </c>
       <c r="B1668">
-        <v>0.7759999999999999</v>
+        <v>0.776</v>
       </c>
     </row>
     <row r="1669" spans="1:2">
@@ -32443,7 +32488,7 @@
         <v>1199</v>
       </c>
       <c r="B1669">
-        <v>0.7759999999999999</v>
+        <v>0.776</v>
       </c>
     </row>
     <row r="1670" spans="1:2">
@@ -32451,7 +32496,7 @@
         <v>1200</v>
       </c>
       <c r="B1670">
-        <v>0.7759999999999999</v>
+        <v>0.776</v>
       </c>
     </row>
     <row r="1671" spans="1:2">
@@ -32459,7 +32504,7 @@
         <v>1200</v>
       </c>
       <c r="B1671">
-        <v>0.7759999999999999</v>
+        <v>0.776</v>
       </c>
     </row>
     <row r="1672" spans="1:2">
@@ -32467,7 +32512,7 @@
         <v>1201</v>
       </c>
       <c r="B1672">
-        <v>0.7759999999999999</v>
+        <v>0.776</v>
       </c>
     </row>
     <row r="1673" spans="1:2">
@@ -32475,7 +32520,7 @@
         <v>1201</v>
       </c>
       <c r="B1673">
-        <v>0.7759999999999999</v>
+        <v>0.776</v>
       </c>
     </row>
     <row r="1674" spans="1:2">
@@ -32483,7 +32528,7 @@
         <v>1202</v>
       </c>
       <c r="B1674">
-        <v>0.7759999999999999</v>
+        <v>0.776</v>
       </c>
     </row>
     <row r="1675" spans="1:2">
@@ -32491,7 +32536,7 @@
         <v>1202</v>
       </c>
       <c r="B1675">
-        <v>0.7759999999999999</v>
+        <v>0.776</v>
       </c>
     </row>
     <row r="1676" spans="1:2">
@@ -32499,7 +32544,7 @@
         <v>1203</v>
       </c>
       <c r="B1676">
-        <v>0.7759999999999999</v>
+        <v>0.776</v>
       </c>
     </row>
     <row r="1677" spans="1:2">
@@ -32507,7 +32552,7 @@
         <v>1203</v>
       </c>
       <c r="B1677">
-        <v>0.7759999999999999</v>
+        <v>0.776</v>
       </c>
     </row>
     <row r="1678" spans="1:2">
@@ -32515,7 +32560,7 @@
         <v>1204</v>
       </c>
       <c r="B1678">
-        <v>0.7759999999999999</v>
+        <v>0.776</v>
       </c>
     </row>
     <row r="1679" spans="1:2">
@@ -32523,7 +32568,7 @@
         <v>1204</v>
       </c>
       <c r="B1679">
-        <v>0.7759999999999999</v>
+        <v>0.776</v>
       </c>
     </row>
     <row r="1680" spans="1:2">
@@ -32531,7 +32576,7 @@
         <v>1205</v>
       </c>
       <c r="B1680">
-        <v>0.7759999999999999</v>
+        <v>0.776</v>
       </c>
     </row>
     <row r="1681" spans="1:2">
@@ -32539,7 +32584,7 @@
         <v>1205</v>
       </c>
       <c r="B1681">
-        <v>0.7759999999999999</v>
+        <v>0.776</v>
       </c>
     </row>
     <row r="1682" spans="1:2">
@@ -32547,7 +32592,7 @@
         <v>1206</v>
       </c>
       <c r="B1682">
-        <v>0.7759999999999999</v>
+        <v>0.776</v>
       </c>
     </row>
     <row r="1683" spans="1:2">
@@ -32555,7 +32600,7 @@
         <v>1206</v>
       </c>
       <c r="B1683">
-        <v>0.7759999999999999</v>
+        <v>0.776</v>
       </c>
     </row>
     <row r="1684" spans="1:2">
@@ -32563,7 +32608,7 @@
         <v>1207</v>
       </c>
       <c r="B1684">
-        <v>0.7759999999999999</v>
+        <v>0.776</v>
       </c>
     </row>
     <row r="1685" spans="1:2">
@@ -32571,7 +32616,7 @@
         <v>1207</v>
       </c>
       <c r="B1685">
-        <v>0.7759999999999999</v>
+        <v>0.776</v>
       </c>
     </row>
     <row r="1686" spans="1:2">
@@ -33315,7 +33360,7 @@
         <v>1254</v>
       </c>
       <c r="B1778">
-        <v>0.7759999999999999</v>
+        <v>0.776</v>
       </c>
     </row>
     <row r="1779" spans="1:2">
@@ -33323,7 +33368,7 @@
         <v>1254</v>
       </c>
       <c r="B1779">
-        <v>0.7759999999999999</v>
+        <v>0.776</v>
       </c>
     </row>
     <row r="1780" spans="1:2">
@@ -33331,7 +33376,7 @@
         <v>1255</v>
       </c>
       <c r="B1780">
-        <v>0.7759999999999999</v>
+        <v>0.776</v>
       </c>
     </row>
     <row r="1781" spans="1:2">
@@ -33339,7 +33384,7 @@
         <v>1255</v>
       </c>
       <c r="B1781">
-        <v>0.7759999999999999</v>
+        <v>0.776</v>
       </c>
     </row>
     <row r="1782" spans="1:2">
@@ -34931,7 +34976,7 @@
         <v>1355</v>
       </c>
       <c r="B1980">
-        <v>0.0559999999999999</v>
+        <v>0.056</v>
       </c>
     </row>
     <row r="1981" spans="1:2">
@@ -34939,7 +34984,7 @@
         <v>1355</v>
       </c>
       <c r="B1981">
-        <v>0.0559999999999999</v>
+        <v>0.056</v>
       </c>
     </row>
     <row r="1982" spans="1:2">
@@ -35395,7 +35440,7 @@
         <v>1384</v>
       </c>
       <c r="B2038">
-        <v>0.2239999999999999</v>
+        <v>0.224</v>
       </c>
     </row>
     <row r="2039" spans="1:2">
@@ -35403,7 +35448,7 @@
         <v>1384</v>
       </c>
       <c r="B2039">
-        <v>0.2239999999999999</v>
+        <v>0.224</v>
       </c>
     </row>
     <row r="2040" spans="1:2">
@@ -35411,7 +35456,7 @@
         <v>1385</v>
       </c>
       <c r="B2040">
-        <v>0.2239999999999999</v>
+        <v>0.224</v>
       </c>
     </row>
     <row r="2041" spans="1:2">
@@ -35419,7 +35464,7 @@
         <v>1385</v>
       </c>
       <c r="B2041">
-        <v>0.2239999999999999</v>
+        <v>0.224</v>
       </c>
     </row>
     <row r="2042" spans="1:2">
@@ -35427,7 +35472,7 @@
         <v>1386</v>
       </c>
       <c r="B2042">
-        <v>0.2239999999999999</v>
+        <v>0.224</v>
       </c>
     </row>
     <row r="2043" spans="1:2">
@@ -35435,7 +35480,7 @@
         <v>1386</v>
       </c>
       <c r="B2043">
-        <v>0.2239999999999999</v>
+        <v>0.224</v>
       </c>
     </row>
     <row r="2044" spans="1:2">
@@ -35443,7 +35488,7 @@
         <v>1387</v>
       </c>
       <c r="B2044">
-        <v>0.2239999999999999</v>
+        <v>0.224</v>
       </c>
     </row>
     <row r="2045" spans="1:2">
@@ -35451,7 +35496,7 @@
         <v>1387</v>
       </c>
       <c r="B2045">
-        <v>0.2239999999999999</v>
+        <v>0.224</v>
       </c>
     </row>
     <row r="2046" spans="1:2">
@@ -35459,7 +35504,7 @@
         <v>1388</v>
       </c>
       <c r="B2046">
-        <v>0.2239999999999999</v>
+        <v>0.224</v>
       </c>
     </row>
     <row r="2047" spans="1:2">
@@ -35467,7 +35512,7 @@
         <v>1388</v>
       </c>
       <c r="B2047">
-        <v>0.2239999999999999</v>
+        <v>0.224</v>
       </c>
     </row>
     <row r="2048" spans="1:2">
@@ -35475,7 +35520,7 @@
         <v>1389</v>
       </c>
       <c r="B2048">
-        <v>0.2239999999999999</v>
+        <v>0.224</v>
       </c>
     </row>
     <row r="2049" spans="1:2">
@@ -35483,7 +35528,7 @@
         <v>1389</v>
       </c>
       <c r="B2049">
-        <v>0.2239999999999999</v>
+        <v>0.224</v>
       </c>
     </row>
     <row r="2050" spans="1:2">
@@ -35491,7 +35536,7 @@
         <v>1390</v>
       </c>
       <c r="B2050">
-        <v>0.2239999999999999</v>
+        <v>0.224</v>
       </c>
     </row>
     <row r="2051" spans="1:2">
@@ -35499,7 +35544,7 @@
         <v>1390</v>
       </c>
       <c r="B2051">
-        <v>0.2239999999999999</v>
+        <v>0.224</v>
       </c>
     </row>
     <row r="2052" spans="1:2">
@@ -35507,7 +35552,7 @@
         <v>1391</v>
       </c>
       <c r="B2052">
-        <v>0.2239999999999999</v>
+        <v>0.224</v>
       </c>
     </row>
     <row r="2053" spans="1:2">
@@ -35515,7 +35560,7 @@
         <v>1391</v>
       </c>
       <c r="B2053">
-        <v>0.2239999999999999</v>
+        <v>0.224</v>
       </c>
     </row>
     <row r="2054" spans="1:2">
@@ -35523,7 +35568,7 @@
         <v>1392</v>
       </c>
       <c r="B2054">
-        <v>0.2239999999999999</v>
+        <v>0.224</v>
       </c>
     </row>
     <row r="2055" spans="1:2">
@@ -35531,7 +35576,7 @@
         <v>1392</v>
       </c>
       <c r="B2055">
-        <v>0.2239999999999999</v>
+        <v>0.224</v>
       </c>
     </row>
     <row r="2056" spans="1:2">
@@ -35539,7 +35584,7 @@
         <v>1393</v>
       </c>
       <c r="B2056">
-        <v>0.2239999999999999</v>
+        <v>0.224</v>
       </c>
     </row>
     <row r="2057" spans="1:2">
@@ -35547,7 +35592,7 @@
         <v>1393</v>
       </c>
       <c r="B2057">
-        <v>0.2239999999999999</v>
+        <v>0.224</v>
       </c>
     </row>
     <row r="2058" spans="1:2">
@@ -35555,7 +35600,7 @@
         <v>1394</v>
       </c>
       <c r="B2058">
-        <v>0.2239999999999999</v>
+        <v>0.224</v>
       </c>
     </row>
     <row r="2059" spans="1:2">
@@ -35563,7 +35608,7 @@
         <v>1394</v>
       </c>
       <c r="B2059">
-        <v>0.2239999999999999</v>
+        <v>0.224</v>
       </c>
     </row>
     <row r="2060" spans="1:2">
@@ -35571,7 +35616,7 @@
         <v>1395</v>
       </c>
       <c r="B2060">
-        <v>0.2239999999999999</v>
+        <v>0.224</v>
       </c>
     </row>
     <row r="2061" spans="1:2">
@@ -35579,7 +35624,7 @@
         <v>1395</v>
       </c>
       <c r="B2061">
-        <v>0.2239999999999999</v>
+        <v>0.224</v>
       </c>
     </row>
     <row r="2062" spans="1:2">
@@ -35587,7 +35632,7 @@
         <v>1396</v>
       </c>
       <c r="B2062">
-        <v>0.2239999999999999</v>
+        <v>0.224</v>
       </c>
     </row>
     <row r="2063" spans="1:2">
@@ -35595,7 +35640,7 @@
         <v>1396</v>
       </c>
       <c r="B2063">
-        <v>0.2239999999999999</v>
+        <v>0.224</v>
       </c>
     </row>
     <row r="2064" spans="1:2">
@@ -35603,7 +35648,7 @@
         <v>1397</v>
       </c>
       <c r="B2064">
-        <v>0.2239999999999999</v>
+        <v>0.224</v>
       </c>
     </row>
     <row r="2065" spans="1:2">
@@ -35611,7 +35656,7 @@
         <v>1397</v>
       </c>
       <c r="B2065">
-        <v>0.2239999999999999</v>
+        <v>0.224</v>
       </c>
     </row>
     <row r="2066" spans="1:2">
@@ -35619,7 +35664,7 @@
         <v>1398</v>
       </c>
       <c r="B2066">
-        <v>0.2239999999999999</v>
+        <v>0.224</v>
       </c>
     </row>
     <row r="2067" spans="1:2">
@@ -35627,7 +35672,7 @@
         <v>1398</v>
       </c>
       <c r="B2067">
-        <v>0.2239999999999999</v>
+        <v>0.224</v>
       </c>
     </row>
     <row r="2068" spans="1:2">
@@ -35635,7 +35680,7 @@
         <v>1399</v>
       </c>
       <c r="B2068">
-        <v>0.2319999999999999</v>
+        <v>0.232</v>
       </c>
     </row>
     <row r="2069" spans="1:2">
@@ -35643,7 +35688,7 @@
         <v>1399</v>
       </c>
       <c r="B2069">
-        <v>0.2319999999999999</v>
+        <v>0.232</v>
       </c>
     </row>
     <row r="2070" spans="1:2">
@@ -36147,7 +36192,7 @@
         <v>1431</v>
       </c>
       <c r="B2132">
-        <v>0.1119999999999999</v>
+        <v>0.112</v>
       </c>
     </row>
     <row r="2133" spans="1:2">
@@ -36155,7 +36200,7 @@
         <v>1431</v>
       </c>
       <c r="B2133">
-        <v>0.1119999999999999</v>
+        <v>0.112</v>
       </c>
     </row>
     <row r="2134" spans="1:2">
@@ -36163,7 +36208,7 @@
         <v>1432</v>
       </c>
       <c r="B2134">
-        <v>0.1119999999999999</v>
+        <v>0.112</v>
       </c>
     </row>
     <row r="2135" spans="1:2">
@@ -36171,7 +36216,7 @@
         <v>1432</v>
       </c>
       <c r="B2135">
-        <v>0.1119999999999999</v>
+        <v>0.112</v>
       </c>
     </row>
     <row r="2136" spans="1:2">
@@ -36179,7 +36224,7 @@
         <v>1433</v>
       </c>
       <c r="B2136">
-        <v>0.1119999999999999</v>
+        <v>0.112</v>
       </c>
     </row>
     <row r="2137" spans="1:2">
@@ -36187,7 +36232,7 @@
         <v>1433</v>
       </c>
       <c r="B2137">
-        <v>0.1119999999999999</v>
+        <v>0.112</v>
       </c>
     </row>
     <row r="2138" spans="1:2">
@@ -36195,7 +36240,7 @@
         <v>1434</v>
       </c>
       <c r="B2138">
-        <v>0.1119999999999999</v>
+        <v>0.112</v>
       </c>
     </row>
     <row r="2139" spans="1:2">
@@ -36203,7 +36248,7 @@
         <v>1434</v>
       </c>
       <c r="B2139">
-        <v>0.1119999999999999</v>
+        <v>0.112</v>
       </c>
     </row>
     <row r="2140" spans="1:2">
@@ -36211,7 +36256,7 @@
         <v>1435</v>
       </c>
       <c r="B2140">
-        <v>0.1119999999999999</v>
+        <v>0.112</v>
       </c>
     </row>
     <row r="2141" spans="1:2">
@@ -36219,7 +36264,7 @@
         <v>1435</v>
       </c>
       <c r="B2141">
-        <v>0.1119999999999999</v>
+        <v>0.112</v>
       </c>
     </row>
     <row r="2142" spans="1:2">
@@ -36227,7 +36272,7 @@
         <v>1436</v>
       </c>
       <c r="B2142">
-        <v>0.1119999999999999</v>
+        <v>0.112</v>
       </c>
     </row>
     <row r="2143" spans="1:2">
@@ -36235,7 +36280,7 @@
         <v>1436</v>
       </c>
       <c r="B2143">
-        <v>0.1119999999999999</v>
+        <v>0.112</v>
       </c>
     </row>
     <row r="2144" spans="1:2">
@@ -36243,7 +36288,7 @@
         <v>1437</v>
       </c>
       <c r="B2144">
-        <v>0.1119999999999999</v>
+        <v>0.112</v>
       </c>
     </row>
     <row r="2145" spans="1:2">
@@ -36251,7 +36296,7 @@
         <v>1437</v>
       </c>
       <c r="B2145">
-        <v>0.1119999999999999</v>
+        <v>0.112</v>
       </c>
     </row>
     <row r="2146" spans="1:2">
@@ -36259,7 +36304,7 @@
         <v>1438</v>
       </c>
       <c r="B2146">
-        <v>0.1119999999999999</v>
+        <v>0.112</v>
       </c>
     </row>
     <row r="2147" spans="1:2">
@@ -36267,7 +36312,7 @@
         <v>1438</v>
       </c>
       <c r="B2147">
-        <v>0.1119999999999999</v>
+        <v>0.112</v>
       </c>
     </row>
     <row r="2148" spans="1:2">
@@ -36275,7 +36320,7 @@
         <v>1439</v>
       </c>
       <c r="B2148">
-        <v>0.1119999999999999</v>
+        <v>0.112</v>
       </c>
     </row>
     <row r="2149" spans="1:2">
@@ -36283,7 +36328,7 @@
         <v>1439</v>
       </c>
       <c r="B2149">
-        <v>0.1119999999999999</v>
+        <v>0.112</v>
       </c>
     </row>
     <row r="2150" spans="1:2">
@@ -36291,7 +36336,7 @@
         <v>1440</v>
       </c>
       <c r="B2150">
-        <v>0.1119999999999999</v>
+        <v>0.112</v>
       </c>
     </row>
     <row r="2151" spans="1:2">
@@ -36299,7 +36344,7 @@
         <v>1440</v>
       </c>
       <c r="B2151">
-        <v>0.1119999999999999</v>
+        <v>0.112</v>
       </c>
     </row>
     <row r="2152" spans="1:2">
@@ -36307,7 +36352,7 @@
         <v>1441</v>
       </c>
       <c r="B2152">
-        <v>0.1119999999999999</v>
+        <v>0.112</v>
       </c>
     </row>
     <row r="2153" spans="1:2">
@@ -36315,7 +36360,7 @@
         <v>1441</v>
       </c>
       <c r="B2153">
-        <v>0.1119999999999999</v>
+        <v>0.112</v>
       </c>
     </row>
     <row r="2154" spans="1:2">
@@ -36323,7 +36368,7 @@
         <v>1442</v>
       </c>
       <c r="B2154">
-        <v>0.1119999999999999</v>
+        <v>0.112</v>
       </c>
     </row>
     <row r="2155" spans="1:2">
@@ -36331,7 +36376,7 @@
         <v>1442</v>
       </c>
       <c r="B2155">
-        <v>0.1119999999999999</v>
+        <v>0.112</v>
       </c>
     </row>
     <row r="2156" spans="1:2">
@@ -36339,7 +36384,7 @@
         <v>1443</v>
       </c>
       <c r="B2156">
-        <v>0.1119999999999999</v>
+        <v>0.112</v>
       </c>
     </row>
     <row r="2157" spans="1:2">
@@ -36347,7 +36392,7 @@
         <v>1443</v>
       </c>
       <c r="B2157">
-        <v>0.1119999999999999</v>
+        <v>0.112</v>
       </c>
     </row>
     <row r="2158" spans="1:2">
@@ -36355,7 +36400,7 @@
         <v>1444</v>
       </c>
       <c r="B2158">
-        <v>0.1119999999999999</v>
+        <v>0.112</v>
       </c>
     </row>
     <row r="2159" spans="1:2">
@@ -36363,7 +36408,7 @@
         <v>1444</v>
       </c>
       <c r="B2159">
-        <v>0.1119999999999999</v>
+        <v>0.112</v>
       </c>
     </row>
     <row r="2160" spans="1:2">
@@ -36371,7 +36416,7 @@
         <v>1445</v>
       </c>
       <c r="B2160">
-        <v>0.1119999999999999</v>
+        <v>0.112</v>
       </c>
     </row>
     <row r="2161" spans="1:2">
@@ -36379,7 +36424,7 @@
         <v>1445</v>
       </c>
       <c r="B2161">
-        <v>0.1119999999999999</v>
+        <v>0.112</v>
       </c>
     </row>
     <row r="2162" spans="1:2">
@@ -36387,7 +36432,7 @@
         <v>1446</v>
       </c>
       <c r="B2162">
-        <v>0.1119999999999999</v>
+        <v>0.112</v>
       </c>
     </row>
     <row r="2163" spans="1:2">
@@ -36395,7 +36440,7 @@
         <v>1446</v>
       </c>
       <c r="B2163">
-        <v>0.1119999999999999</v>
+        <v>0.112</v>
       </c>
     </row>
     <row r="2164" spans="1:2">
@@ -37235,7 +37280,7 @@
         <v>1499</v>
       </c>
       <c r="B2268">
-        <v>0.0559999999999999</v>
+        <v>0.056</v>
       </c>
     </row>
     <row r="2269" spans="1:2">
@@ -37243,7 +37288,7 @@
         <v>1499</v>
       </c>
       <c r="B2269">
-        <v>0.0559999999999999</v>
+        <v>0.056</v>
       </c>
     </row>
     <row r="2270" spans="1:2">
@@ -41379,7 +41424,7 @@
         <v>1758</v>
       </c>
       <c r="B2786">
-        <v>0.1119999999999999</v>
+        <v>0.112</v>
       </c>
     </row>
     <row r="2787" spans="1:2">
@@ -41387,7 +41432,7 @@
         <v>1758</v>
       </c>
       <c r="B2787">
-        <v>0.1119999999999999</v>
+        <v>0.112</v>
       </c>
     </row>
     <row r="2788" spans="1:2">
@@ -44451,7 +44496,7 @@
         <v>1950</v>
       </c>
       <c r="B3170">
-        <v>0.0559999999999999</v>
+        <v>0.056</v>
       </c>
     </row>
     <row r="3171" spans="1:2">
@@ -44459,7 +44504,7 @@
         <v>1950</v>
       </c>
       <c r="B3171">
-        <v>0.0559999999999999</v>
+        <v>0.056</v>
       </c>
     </row>
     <row r="3172" spans="1:2">
@@ -44467,7 +44512,7 @@
         <v>1951</v>
       </c>
       <c r="B3172">
-        <v>0.0559999999999999</v>
+        <v>0.056</v>
       </c>
     </row>
     <row r="3173" spans="1:2">
@@ -44475,7 +44520,7 @@
         <v>1951</v>
       </c>
       <c r="B3173">
-        <v>0.0559999999999999</v>
+        <v>0.056</v>
       </c>
     </row>
     <row r="3174" spans="1:2">
@@ -45267,7 +45312,7 @@
         <v>2001</v>
       </c>
       <c r="B3272">
-        <v>0.1119999999999999</v>
+        <v>0.112</v>
       </c>
     </row>
     <row r="3273" spans="1:2">
@@ -45275,7 +45320,7 @@
         <v>2001</v>
       </c>
       <c r="B3273">
-        <v>0.1119999999999999</v>
+        <v>0.112</v>
       </c>
     </row>
     <row r="3274" spans="1:2">
@@ -46243,7 +46288,7 @@
         <v>2062</v>
       </c>
       <c r="B3394">
-        <v>0.0559999999999999</v>
+        <v>0.056</v>
       </c>
     </row>
     <row r="3395" spans="1:2">
@@ -46251,7 +46296,7 @@
         <v>2062</v>
       </c>
       <c r="B3395">
-        <v>0.0559999999999999</v>
+        <v>0.056</v>
       </c>
     </row>
     <row r="3396" spans="1:2">
@@ -46259,7 +46304,7 @@
         <v>2063</v>
       </c>
       <c r="B3396">
-        <v>0.0559999999999999</v>
+        <v>0.056</v>
       </c>
     </row>
     <row r="3397" spans="1:2">
@@ -46267,7 +46312,7 @@
         <v>2063</v>
       </c>
       <c r="B3397">
-        <v>0.0559999999999999</v>
+        <v>0.056</v>
       </c>
     </row>
     <row r="3398" spans="1:2">
@@ -46275,7 +46320,7 @@
         <v>2064</v>
       </c>
       <c r="B3398">
-        <v>0.0559999999999999</v>
+        <v>0.056</v>
       </c>
     </row>
     <row r="3399" spans="1:2">
@@ -46283,7 +46328,7 @@
         <v>2064</v>
       </c>
       <c r="B3399">
-        <v>0.0559999999999999</v>
+        <v>0.056</v>
       </c>
     </row>
     <row r="3400" spans="1:2">
@@ -46291,7 +46336,7 @@
         <v>2065</v>
       </c>
       <c r="B3400">
-        <v>0.0559999999999999</v>
+        <v>0.056</v>
       </c>
     </row>
     <row r="3401" spans="1:2">
@@ -46299,7 +46344,7 @@
         <v>2065</v>
       </c>
       <c r="B3401">
-        <v>0.0559999999999999</v>
+        <v>0.056</v>
       </c>
     </row>
     <row r="3402" spans="1:2">
@@ -46307,7 +46352,7 @@
         <v>2066</v>
       </c>
       <c r="B3402">
-        <v>0.0559999999999999</v>
+        <v>0.056</v>
       </c>
     </row>
     <row r="3403" spans="1:2">
@@ -46315,7 +46360,7 @@
         <v>2066</v>
       </c>
       <c r="B3403">
-        <v>0.0559999999999999</v>
+        <v>0.056</v>
       </c>
     </row>
     <row r="3404" spans="1:2">
@@ -46323,7 +46368,7 @@
         <v>2067</v>
       </c>
       <c r="B3404">
-        <v>0.0559999999999999</v>
+        <v>0.056</v>
       </c>
     </row>
     <row r="3405" spans="1:2">
@@ -46331,7 +46376,7 @@
         <v>2067</v>
       </c>
       <c r="B3405">
-        <v>0.0559999999999999</v>
+        <v>0.056</v>
       </c>
     </row>
     <row r="3406" spans="1:2">
@@ -46835,7 +46880,7 @@
         <v>2099</v>
       </c>
       <c r="B3468">
-        <v>0.1119999999999999</v>
+        <v>0.112</v>
       </c>
     </row>
     <row r="3469" spans="1:2">
@@ -46843,7 +46888,7 @@
         <v>2099</v>
       </c>
       <c r="B3469">
-        <v>0.1119999999999999</v>
+        <v>0.112</v>
       </c>
     </row>
     <row r="3470" spans="1:2">
@@ -46851,7 +46896,7 @@
         <v>2100</v>
       </c>
       <c r="B3470">
-        <v>0.1119999999999999</v>
+        <v>0.112</v>
       </c>
     </row>
     <row r="3471" spans="1:2">
@@ -46859,7 +46904,7 @@
         <v>2100</v>
       </c>
       <c r="B3471">
-        <v>0.1119999999999999</v>
+        <v>0.112</v>
       </c>
     </row>
     <row r="3472" spans="1:2">
@@ -50531,7 +50576,7 @@
         <v>2330</v>
       </c>
       <c r="B3930">
-        <v>0.0559999999999999</v>
+        <v>0.056</v>
       </c>
     </row>
     <row r="3931" spans="1:2">
@@ -50539,7 +50584,7 @@
         <v>2330</v>
       </c>
       <c r="B3931">
-        <v>0.0559999999999999</v>
+        <v>0.056</v>
       </c>
     </row>
     <row r="3932" spans="1:2">
@@ -50547,7 +50592,7 @@
         <v>2331</v>
       </c>
       <c r="B3932">
-        <v>0.0559999999999999</v>
+        <v>0.056</v>
       </c>
     </row>
     <row r="3933" spans="1:2">
@@ -50555,7 +50600,7 @@
         <v>2331</v>
       </c>
       <c r="B3933">
-        <v>0.0559999999999999</v>
+        <v>0.056</v>
       </c>
     </row>
     <row r="3934" spans="1:2">
@@ -53347,7 +53392,7 @@
         <v>2506</v>
       </c>
       <c r="B4282">
-        <v>0.4639999999999999</v>
+        <v>0.464</v>
       </c>
     </row>
     <row r="4283" spans="1:2">
@@ -53355,7 +53400,7 @@
         <v>2506</v>
       </c>
       <c r="B4283">
-        <v>0.4639999999999999</v>
+        <v>0.464</v>
       </c>
     </row>
     <row r="4284" spans="1:2">
@@ -53795,7 +53840,7 @@
         <v>2534</v>
       </c>
       <c r="B4338">
-        <v>0.8959999999999999</v>
+        <v>0.896</v>
       </c>
     </row>
     <row r="4339" spans="1:2">
@@ -53803,7 +53848,7 @@
         <v>2534</v>
       </c>
       <c r="B4339">
-        <v>0.8959999999999999</v>
+        <v>0.896</v>
       </c>
     </row>
     <row r="4340" spans="1:2">
@@ -53811,7 +53856,7 @@
         <v>2535</v>
       </c>
       <c r="B4340">
-        <v>0.8959999999999999</v>
+        <v>0.896</v>
       </c>
     </row>
     <row r="4341" spans="1:2">
@@ -53819,7 +53864,7 @@
         <v>2535</v>
       </c>
       <c r="B4341">
-        <v>0.8959999999999999</v>
+        <v>0.896</v>
       </c>
     </row>
     <row r="4342" spans="1:2">
@@ -54451,7 +54496,7 @@
         <v>2575</v>
       </c>
       <c r="B4420">
-        <v>0.6559999999999999</v>
+        <v>0.656</v>
       </c>
     </row>
     <row r="4421" spans="1:2">
@@ -54459,7 +54504,7 @@
         <v>2575</v>
       </c>
       <c r="B4421">
-        <v>0.6559999999999999</v>
+        <v>0.656</v>
       </c>
     </row>
     <row r="4422" spans="1:2">
@@ -54467,7 +54512,7 @@
         <v>2576</v>
       </c>
       <c r="B4422">
-        <v>0.6559999999999999</v>
+        <v>0.656</v>
       </c>
     </row>
     <row r="4423" spans="1:2">
@@ -54475,7 +54520,7 @@
         <v>2576</v>
       </c>
       <c r="B4423">
-        <v>0.6559999999999999</v>
+        <v>0.656</v>
       </c>
     </row>
     <row r="4424" spans="1:2">
@@ -54483,7 +54528,7 @@
         <v>2577</v>
       </c>
       <c r="B4424">
-        <v>0.6559999999999999</v>
+        <v>0.656</v>
       </c>
     </row>
     <row r="4425" spans="1:2">
@@ -54491,7 +54536,7 @@
         <v>2577</v>
       </c>
       <c r="B4425">
-        <v>0.6559999999999999</v>
+        <v>0.656</v>
       </c>
     </row>
     <row r="4426" spans="1:2">
@@ -54499,7 +54544,7 @@
         <v>2578</v>
       </c>
       <c r="B4426">
-        <v>0.6559999999999999</v>
+        <v>0.656</v>
       </c>
     </row>
     <row r="4427" spans="1:2">
@@ -54507,7 +54552,7 @@
         <v>2578</v>
       </c>
       <c r="B4427">
-        <v>0.6559999999999999</v>
+        <v>0.656</v>
       </c>
     </row>
     <row r="4428" spans="1:2">
@@ -54515,7 +54560,7 @@
         <v>2579</v>
       </c>
       <c r="B4428">
-        <v>0.6559999999999999</v>
+        <v>0.656</v>
       </c>
     </row>
     <row r="4429" spans="1:2">
@@ -54523,7 +54568,7 @@
         <v>2579</v>
       </c>
       <c r="B4429">
-        <v>0.6559999999999999</v>
+        <v>0.656</v>
       </c>
     </row>
     <row r="4430" spans="1:2">
@@ -54531,7 +54576,7 @@
         <v>2580</v>
       </c>
       <c r="B4430">
-        <v>0.6559999999999999</v>
+        <v>0.656</v>
       </c>
     </row>
     <row r="4431" spans="1:2">
@@ -54539,7 +54584,7 @@
         <v>2580</v>
       </c>
       <c r="B4431">
-        <v>0.6559999999999999</v>
+        <v>0.656</v>
       </c>
     </row>
     <row r="4432" spans="1:2">
@@ -54979,7 +55024,7 @@
         <v>2608</v>
       </c>
       <c r="B4486">
-        <v>0.1119999999999999</v>
+        <v>0.112</v>
       </c>
     </row>
     <row r="4487" spans="1:2">
@@ -54987,7 +55032,7 @@
         <v>2608</v>
       </c>
       <c r="B4487">
-        <v>0.1119999999999999</v>
+        <v>0.112</v>
       </c>
     </row>
     <row r="4488" spans="1:2">
@@ -54995,7 +55040,7 @@
         <v>2609</v>
       </c>
       <c r="B4488">
-        <v>0.1119999999999999</v>
+        <v>0.112</v>
       </c>
     </row>
     <row r="4489" spans="1:2">
@@ -55003,7 +55048,7 @@
         <v>2609</v>
       </c>
       <c r="B4489">
-        <v>0.1119999999999999</v>
+        <v>0.112</v>
       </c>
     </row>
     <row r="4490" spans="1:2">
@@ -55987,7 +56032,7 @@
         <v>159</v>
       </c>
       <c r="B4612">
-        <v>0.1119999999999999</v>
+        <v>0.112</v>
       </c>
     </row>
     <row r="4613" spans="1:2">
@@ -55995,7 +56040,7 @@
         <v>159</v>
       </c>
       <c r="B4613">
-        <v>0.1119999999999999</v>
+        <v>0.112</v>
       </c>
     </row>
     <row r="4614" spans="1:2">
@@ -56003,7 +56048,7 @@
         <v>160</v>
       </c>
       <c r="B4614">
-        <v>0.1119999999999999</v>
+        <v>0.112</v>
       </c>
     </row>
     <row r="4615" spans="1:2">
@@ -56011,7 +56056,7 @@
         <v>160</v>
       </c>
       <c r="B4615">
-        <v>0.1119999999999999</v>
+        <v>0.112</v>
       </c>
     </row>
     <row r="4616" spans="1:2">
@@ -56019,7 +56064,7 @@
         <v>161</v>
       </c>
       <c r="B4616">
-        <v>0.1119999999999999</v>
+        <v>0.112</v>
       </c>
     </row>
     <row r="4617" spans="1:2">
@@ -56027,7 +56072,7 @@
         <v>161</v>
       </c>
       <c r="B4617">
-        <v>0.1119999999999999</v>
+        <v>0.112</v>
       </c>
     </row>
     <row r="4618" spans="1:2">
@@ -56883,7 +56928,7 @@
         <v>358</v>
       </c>
       <c r="B4724">
-        <v>0.3279999999999999</v>
+        <v>0.328</v>
       </c>
     </row>
     <row r="4725" spans="1:2">
@@ -56891,7 +56936,7 @@
         <v>358</v>
       </c>
       <c r="B4725">
-        <v>0.3279999999999999</v>
+        <v>0.328</v>
       </c>
     </row>
     <row r="4726" spans="1:2">
@@ -56899,7 +56944,7 @@
         <v>359</v>
       </c>
       <c r="B4726">
-        <v>0.3279999999999999</v>
+        <v>0.328</v>
       </c>
     </row>
     <row r="4727" spans="1:2">
@@ -56907,7 +56952,7 @@
         <v>359</v>
       </c>
       <c r="B4727">
-        <v>0.3279999999999999</v>
+        <v>0.328</v>
       </c>
     </row>
     <row r="4728" spans="1:2">
@@ -56915,7 +56960,7 @@
         <v>360</v>
       </c>
       <c r="B4728">
-        <v>0.3279999999999999</v>
+        <v>0.328</v>
       </c>
     </row>
     <row r="4729" spans="1:2">
@@ -56923,7 +56968,7 @@
         <v>360</v>
       </c>
       <c r="B4729">
-        <v>0.3279999999999999</v>
+        <v>0.328</v>
       </c>
     </row>
     <row r="4730" spans="1:2">
@@ -56931,7 +56976,7 @@
         <v>361</v>
       </c>
       <c r="B4730">
-        <v>0.3279999999999999</v>
+        <v>0.328</v>
       </c>
     </row>
     <row r="4731" spans="1:2">
@@ -56939,7 +56984,7 @@
         <v>361</v>
       </c>
       <c r="B4731">
-        <v>0.3279999999999999</v>
+        <v>0.328</v>
       </c>
     </row>
     <row r="4732" spans="1:2">
@@ -56947,7 +56992,7 @@
         <v>362</v>
       </c>
       <c r="B4732">
-        <v>0.3279999999999999</v>
+        <v>0.328</v>
       </c>
     </row>
     <row r="4733" spans="1:2">
@@ -56955,7 +57000,7 @@
         <v>362</v>
       </c>
       <c r="B4733">
-        <v>0.3279999999999999</v>
+        <v>0.328</v>
       </c>
     </row>
     <row r="4734" spans="1:2">
@@ -56963,7 +57008,7 @@
         <v>363</v>
       </c>
       <c r="B4734">
-        <v>0.3279999999999999</v>
+        <v>0.328</v>
       </c>
     </row>
     <row r="4735" spans="1:2">
@@ -56971,7 +57016,7 @@
         <v>363</v>
       </c>
       <c r="B4735">
-        <v>0.3279999999999999</v>
+        <v>0.328</v>
       </c>
     </row>
     <row r="4736" spans="1:2">
@@ -56979,7 +57024,7 @@
         <v>364</v>
       </c>
       <c r="B4736">
-        <v>0.3279999999999999</v>
+        <v>0.328</v>
       </c>
     </row>
     <row r="4737" spans="1:2">
@@ -56987,7 +57032,7 @@
         <v>364</v>
       </c>
       <c r="B4737">
-        <v>0.3279999999999999</v>
+        <v>0.328</v>
       </c>
     </row>
     <row r="4738" spans="1:2">
@@ -56995,7 +57040,7 @@
         <v>365</v>
       </c>
       <c r="B4738">
-        <v>0.3279999999999999</v>
+        <v>0.328</v>
       </c>
     </row>
     <row r="4739" spans="1:2">
@@ -57003,7 +57048,7 @@
         <v>365</v>
       </c>
       <c r="B4739">
-        <v>0.3279999999999999</v>
+        <v>0.328</v>
       </c>
     </row>
     <row r="4740" spans="1:2">
@@ -57011,7 +57056,7 @@
         <v>366</v>
       </c>
       <c r="B4740">
-        <v>0.3279999999999999</v>
+        <v>0.328</v>
       </c>
     </row>
     <row r="4741" spans="1:2">
@@ -57019,7 +57064,7 @@
         <v>366</v>
       </c>
       <c r="B4741">
-        <v>0.3279999999999999</v>
+        <v>0.328</v>
       </c>
     </row>
     <row r="4742" spans="1:2">
@@ -57027,7 +57072,7 @@
         <v>2650</v>
       </c>
       <c r="B4742">
-        <v>0.3279999999999999</v>
+        <v>0.328</v>
       </c>
     </row>
     <row r="4743" spans="1:2">
@@ -57035,7 +57080,7 @@
         <v>2650</v>
       </c>
       <c r="B4743">
-        <v>0.3279999999999999</v>
+        <v>0.328</v>
       </c>
     </row>
     <row r="4744" spans="1:2">
@@ -57043,7 +57088,7 @@
         <v>367</v>
       </c>
       <c r="B4744">
-        <v>0.3279999999999999</v>
+        <v>0.328</v>
       </c>
     </row>
     <row r="4745" spans="1:2">
@@ -57051,7 +57096,7 @@
         <v>367</v>
       </c>
       <c r="B4745">
-        <v>0.3279999999999999</v>
+        <v>0.328</v>
       </c>
     </row>
     <row r="4746" spans="1:2">
@@ -57059,7 +57104,7 @@
         <v>368</v>
       </c>
       <c r="B4746">
-        <v>0.3279999999999999</v>
+        <v>0.328</v>
       </c>
     </row>
     <row r="4747" spans="1:2">
@@ -57067,7 +57112,7 @@
         <v>368</v>
       </c>
       <c r="B4747">
-        <v>0.3279999999999999</v>
+        <v>0.328</v>
       </c>
     </row>
     <row r="4748" spans="1:2">
@@ -57075,7 +57120,7 @@
         <v>369</v>
       </c>
       <c r="B4748">
-        <v>0.3279999999999999</v>
+        <v>0.328</v>
       </c>
     </row>
     <row r="4749" spans="1:2">
@@ -57083,7 +57128,7 @@
         <v>369</v>
       </c>
       <c r="B4749">
-        <v>0.3279999999999999</v>
+        <v>0.328</v>
       </c>
     </row>
     <row r="4750" spans="1:2">
@@ -57091,7 +57136,7 @@
         <v>370</v>
       </c>
       <c r="B4750">
-        <v>0.3279999999999999</v>
+        <v>0.328</v>
       </c>
     </row>
     <row r="4751" spans="1:2">
@@ -57099,7 +57144,7 @@
         <v>370</v>
       </c>
       <c r="B4751">
-        <v>0.3279999999999999</v>
+        <v>0.328</v>
       </c>
     </row>
     <row r="4752" spans="1:2">
@@ -58195,7 +58240,7 @@
         <v>439</v>
       </c>
       <c r="B4888">
-        <v>0.1119999999999999</v>
+        <v>0.112</v>
       </c>
     </row>
     <row r="4889" spans="1:2">
@@ -58203,7 +58248,7 @@
         <v>439</v>
       </c>
       <c r="B4889">
-        <v>0.1119999999999999</v>
+        <v>0.112</v>
       </c>
     </row>
     <row r="4890" spans="1:2">
@@ -58764,6 +58809,246 @@
       </c>
       <c r="B4959">
         <v>0.08799999999999999</v>
+      </c>
+    </row>
+    <row r="4960" spans="1:2">
+      <c r="A4960" s="1" t="s">
+        <v>2651</v>
+      </c>
+      <c r="B4960">
+        <v>0.064</v>
+      </c>
+    </row>
+    <row r="4961" spans="1:2">
+      <c r="A4961" s="1" t="s">
+        <v>2651</v>
+      </c>
+      <c r="B4961">
+        <v>0.32</v>
+      </c>
+    </row>
+    <row r="4962" spans="1:2">
+      <c r="A4962" s="1" t="s">
+        <v>2652</v>
+      </c>
+      <c r="B4962">
+        <v>0.064</v>
+      </c>
+    </row>
+    <row r="4963" spans="1:2">
+      <c r="A4963" s="1" t="s">
+        <v>2652</v>
+      </c>
+      <c r="B4963">
+        <v>0.32</v>
+      </c>
+    </row>
+    <row r="4964" spans="1:2">
+      <c r="A4964" s="1" t="s">
+        <v>2653</v>
+      </c>
+      <c r="B4964">
+        <v>0.064</v>
+      </c>
+    </row>
+    <row r="4965" spans="1:2">
+      <c r="A4965" s="1" t="s">
+        <v>2653</v>
+      </c>
+      <c r="B4965">
+        <v>0.32</v>
+      </c>
+    </row>
+    <row r="4966" spans="1:2">
+      <c r="A4966" s="1" t="s">
+        <v>2654</v>
+      </c>
+      <c r="B4966">
+        <v>0.064</v>
+      </c>
+    </row>
+    <row r="4967" spans="1:2">
+      <c r="A4967" s="1" t="s">
+        <v>2654</v>
+      </c>
+      <c r="B4967">
+        <v>0.32</v>
+      </c>
+    </row>
+    <row r="4968" spans="1:2">
+      <c r="A4968" s="1" t="s">
+        <v>2655</v>
+      </c>
+      <c r="B4968">
+        <v>0.064</v>
+      </c>
+    </row>
+    <row r="4969" spans="1:2">
+      <c r="A4969" s="1" t="s">
+        <v>2655</v>
+      </c>
+      <c r="B4969">
+        <v>0.32</v>
+      </c>
+    </row>
+    <row r="4970" spans="1:2">
+      <c r="A4970" s="1" t="s">
+        <v>2656</v>
+      </c>
+      <c r="B4970">
+        <v>0.064</v>
+      </c>
+    </row>
+    <row r="4971" spans="1:2">
+      <c r="A4971" s="1" t="s">
+        <v>2656</v>
+      </c>
+      <c r="B4971">
+        <v>0.32</v>
+      </c>
+    </row>
+    <row r="4972" spans="1:2">
+      <c r="A4972" s="1" t="s">
+        <v>2657</v>
+      </c>
+      <c r="B4972">
+        <v>0.064</v>
+      </c>
+    </row>
+    <row r="4973" spans="1:2">
+      <c r="A4973" s="1" t="s">
+        <v>2657</v>
+      </c>
+      <c r="B4973">
+        <v>0.32</v>
+      </c>
+    </row>
+    <row r="4974" spans="1:2">
+      <c r="A4974" s="1" t="s">
+        <v>2658</v>
+      </c>
+      <c r="B4974">
+        <v>0.064</v>
+      </c>
+    </row>
+    <row r="4975" spans="1:2">
+      <c r="A4975" s="1" t="s">
+        <v>2658</v>
+      </c>
+      <c r="B4975">
+        <v>0.32</v>
+      </c>
+    </row>
+    <row r="4976" spans="1:2">
+      <c r="A4976" s="1" t="s">
+        <v>2659</v>
+      </c>
+      <c r="B4976">
+        <v>0.064</v>
+      </c>
+    </row>
+    <row r="4977" spans="1:2">
+      <c r="A4977" s="1" t="s">
+        <v>2659</v>
+      </c>
+      <c r="B4977">
+        <v>0.32</v>
+      </c>
+    </row>
+    <row r="4978" spans="1:2">
+      <c r="A4978" s="1" t="s">
+        <v>2660</v>
+      </c>
+      <c r="B4978">
+        <v>0.064</v>
+      </c>
+    </row>
+    <row r="4979" spans="1:2">
+      <c r="A4979" s="1" t="s">
+        <v>2660</v>
+      </c>
+      <c r="B4979">
+        <v>0.32</v>
+      </c>
+    </row>
+    <row r="4980" spans="1:2">
+      <c r="A4980" s="1" t="s">
+        <v>2661</v>
+      </c>
+      <c r="B4980">
+        <v>0.064</v>
+      </c>
+    </row>
+    <row r="4981" spans="1:2">
+      <c r="A4981" s="1" t="s">
+        <v>2661</v>
+      </c>
+      <c r="B4981">
+        <v>0.32</v>
+      </c>
+    </row>
+    <row r="4982" spans="1:2">
+      <c r="A4982" s="1" t="s">
+        <v>2662</v>
+      </c>
+      <c r="B4982">
+        <v>0.064</v>
+      </c>
+    </row>
+    <row r="4983" spans="1:2">
+      <c r="A4983" s="1" t="s">
+        <v>2662</v>
+      </c>
+      <c r="B4983">
+        <v>0.32</v>
+      </c>
+    </row>
+    <row r="4984" spans="1:2">
+      <c r="A4984" s="1" t="s">
+        <v>2663</v>
+      </c>
+      <c r="B4984">
+        <v>0.064</v>
+      </c>
+    </row>
+    <row r="4985" spans="1:2">
+      <c r="A4985" s="1" t="s">
+        <v>2663</v>
+      </c>
+      <c r="B4985">
+        <v>0.32</v>
+      </c>
+    </row>
+    <row r="4986" spans="1:2">
+      <c r="A4986" s="1" t="s">
+        <v>2664</v>
+      </c>
+      <c r="B4986">
+        <v>0.064</v>
+      </c>
+    </row>
+    <row r="4987" spans="1:2">
+      <c r="A4987" s="1" t="s">
+        <v>2664</v>
+      </c>
+      <c r="B4987">
+        <v>0.32</v>
+      </c>
+    </row>
+    <row r="4988" spans="1:2">
+      <c r="A4988" s="1" t="s">
+        <v>2665</v>
+      </c>
+      <c r="B4988">
+        <v>0.064</v>
+      </c>
+    </row>
+    <row r="4989" spans="1:2">
+      <c r="A4989" s="1" t="s">
+        <v>2665</v>
+      </c>
+      <c r="B4989">
+        <v>0.32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New Draft for Tagoloan
</commit_message>
<xml_diff>
--- a/Cleaned_Tagoloan/Duplicated Values.xlsx
+++ b/Cleaned_Tagoloan/Duplicated Values.xlsx
@@ -17115,7 +17115,7 @@
         <v>88</v>
       </c>
       <c r="B134">
-        <v>5.4</v>
+        <v>824.8000000000001</v>
       </c>
     </row>
     <row r="135" spans="1:2">
@@ -17131,7 +17131,7 @@
         <v>89</v>
       </c>
       <c r="B136">
-        <v>5.4</v>
+        <v>824.8000000000001</v>
       </c>
     </row>
     <row r="137" spans="1:2">
@@ -17147,7 +17147,7 @@
         <v>90</v>
       </c>
       <c r="B138">
-        <v>5.4</v>
+        <v>824.8000000000001</v>
       </c>
     </row>
     <row r="139" spans="1:2">
@@ -17163,7 +17163,7 @@
         <v>91</v>
       </c>
       <c r="B140">
-        <v>5.4</v>
+        <v>824.8000000000001</v>
       </c>
     </row>
     <row r="141" spans="1:2">
@@ -17179,7 +17179,7 @@
         <v>92</v>
       </c>
       <c r="B142">
-        <v>5.4</v>
+        <v>824.8000000000001</v>
       </c>
     </row>
     <row r="143" spans="1:2">
@@ -17195,7 +17195,7 @@
         <v>93</v>
       </c>
       <c r="B144">
-        <v>5.4</v>
+        <v>824.8000000000001</v>
       </c>
     </row>
     <row r="145" spans="1:2">
@@ -17211,7 +17211,7 @@
         <v>94</v>
       </c>
       <c r="B146">
-        <v>5.4</v>
+        <v>824.8000000000001</v>
       </c>
     </row>
     <row r="147" spans="1:2">
@@ -17227,7 +17227,7 @@
         <v>95</v>
       </c>
       <c r="B148">
-        <v>5.4</v>
+        <v>824.8000000000001</v>
       </c>
     </row>
     <row r="149" spans="1:2">
@@ -17243,7 +17243,7 @@
         <v>96</v>
       </c>
       <c r="B150">
-        <v>5.4</v>
+        <v>824.8000000000001</v>
       </c>
     </row>
     <row r="151" spans="1:2">
@@ -17931,7 +17931,7 @@
         <v>140</v>
       </c>
       <c r="B236">
-        <v>658.2</v>
+        <v>1481</v>
       </c>
     </row>
     <row r="237" spans="1:2">
@@ -17947,7 +17947,7 @@
         <v>141</v>
       </c>
       <c r="B238">
-        <v>658.2</v>
+        <v>1481</v>
       </c>
     </row>
     <row r="239" spans="1:2">
@@ -17963,7 +17963,7 @@
         <v>142</v>
       </c>
       <c r="B240">
-        <v>658.2</v>
+        <v>1481</v>
       </c>
     </row>
     <row r="241" spans="1:2">
@@ -17979,7 +17979,7 @@
         <v>143</v>
       </c>
       <c r="B242">
-        <v>658.2</v>
+        <v>1481</v>
       </c>
     </row>
     <row r="243" spans="1:2">
@@ -17995,7 +17995,7 @@
         <v>144</v>
       </c>
       <c r="B244">
-        <v>658.2</v>
+        <v>1481</v>
       </c>
     </row>
     <row r="245" spans="1:2">
@@ -18011,7 +18011,7 @@
         <v>145</v>
       </c>
       <c r="B246">
-        <v>658.2</v>
+        <v>1481</v>
       </c>
     </row>
     <row r="247" spans="1:2">
@@ -18027,7 +18027,7 @@
         <v>146</v>
       </c>
       <c r="B248">
-        <v>658.2</v>
+        <v>1481</v>
       </c>
     </row>
     <row r="249" spans="1:2">
@@ -18043,7 +18043,7 @@
         <v>147</v>
       </c>
       <c r="B250">
-        <v>658.2</v>
+        <v>1481</v>
       </c>
     </row>
     <row r="251" spans="1:2">
@@ -18059,7 +18059,7 @@
         <v>148</v>
       </c>
       <c r="B252">
-        <v>658.2</v>
+        <v>1481</v>
       </c>
     </row>
     <row r="253" spans="1:2">
@@ -18075,7 +18075,7 @@
         <v>149</v>
       </c>
       <c r="B254">
-        <v>658.2</v>
+        <v>1481</v>
       </c>
     </row>
     <row r="255" spans="1:2">
@@ -18091,7 +18091,7 @@
         <v>150</v>
       </c>
       <c r="B256">
-        <v>658.2</v>
+        <v>1481</v>
       </c>
     </row>
     <row r="257" spans="1:2">
@@ -18107,7 +18107,7 @@
         <v>151</v>
       </c>
       <c r="B258">
-        <v>658.2</v>
+        <v>1481</v>
       </c>
     </row>
     <row r="259" spans="1:2">
@@ -18123,7 +18123,7 @@
         <v>152</v>
       </c>
       <c r="B260">
-        <v>658.2</v>
+        <v>1481</v>
       </c>
     </row>
     <row r="261" spans="1:2">
@@ -18139,7 +18139,7 @@
         <v>153</v>
       </c>
       <c r="B262">
-        <v>658.2</v>
+        <v>1481</v>
       </c>
     </row>
     <row r="263" spans="1:2">
@@ -18155,7 +18155,7 @@
         <v>154</v>
       </c>
       <c r="B264">
-        <v>658.2</v>
+        <v>1481</v>
       </c>
     </row>
     <row r="265" spans="1:2">
@@ -18171,7 +18171,7 @@
         <v>155</v>
       </c>
       <c r="B266">
-        <v>658.2</v>
+        <v>1481</v>
       </c>
     </row>
     <row r="267" spans="1:2">
@@ -18187,7 +18187,7 @@
         <v>156</v>
       </c>
       <c r="B268">
-        <v>658.2</v>
+        <v>1481</v>
       </c>
     </row>
     <row r="269" spans="1:2">
@@ -18203,7 +18203,7 @@
         <v>157</v>
       </c>
       <c r="B270">
-        <v>352.4</v>
+        <v>1182.4</v>
       </c>
     </row>
     <row r="271" spans="1:2">
@@ -18219,7 +18219,7 @@
         <v>158</v>
       </c>
       <c r="B272">
-        <v>352.8</v>
+        <v>1182.8</v>
       </c>
     </row>
     <row r="273" spans="1:2">
@@ -18235,7 +18235,7 @@
         <v>159</v>
       </c>
       <c r="B274">
-        <v>355.2</v>
+        <v>1185.2</v>
       </c>
     </row>
     <row r="275" spans="1:2">
@@ -18251,7 +18251,7 @@
         <v>160</v>
       </c>
       <c r="B276">
-        <v>355.2</v>
+        <v>1185.2</v>
       </c>
     </row>
     <row r="277" spans="1:2">
@@ -18267,7 +18267,7 @@
         <v>161</v>
       </c>
       <c r="B278">
-        <v>355.2</v>
+        <v>1185.2</v>
       </c>
     </row>
     <row r="279" spans="1:2">
@@ -18283,7 +18283,7 @@
         <v>162</v>
       </c>
       <c r="B280">
-        <v>355.4</v>
+        <v>1185.4</v>
       </c>
     </row>
     <row r="281" spans="1:2">
@@ -18299,7 +18299,7 @@
         <v>163</v>
       </c>
       <c r="B282">
-        <v>355.4</v>
+        <v>1185.4</v>
       </c>
     </row>
     <row r="283" spans="1:2">
@@ -18315,7 +18315,7 @@
         <v>164</v>
       </c>
       <c r="B284">
-        <v>355.4</v>
+        <v>1185.4</v>
       </c>
     </row>
     <row r="285" spans="1:2">
@@ -18331,7 +18331,7 @@
         <v>165</v>
       </c>
       <c r="B286">
-        <v>355.4</v>
+        <v>1185.4</v>
       </c>
     </row>
     <row r="287" spans="1:2">
@@ -18347,7 +18347,7 @@
         <v>166</v>
       </c>
       <c r="B288">
-        <v>355.4</v>
+        <v>1185.4</v>
       </c>
     </row>
     <row r="289" spans="1:2">
@@ -18747,7 +18747,7 @@
         <v>453</v>
       </c>
       <c r="B338">
-        <v>124.8</v>
+        <v>946.2</v>
       </c>
     </row>
     <row r="339" spans="1:2">
@@ -18763,7 +18763,7 @@
         <v>454</v>
       </c>
       <c r="B340">
-        <v>124.8</v>
+        <v>946.2</v>
       </c>
     </row>
     <row r="341" spans="1:2">
@@ -18779,7 +18779,7 @@
         <v>455</v>
       </c>
       <c r="B342">
-        <v>124.8</v>
+        <v>946.2</v>
       </c>
     </row>
     <row r="343" spans="1:2">
@@ -18795,7 +18795,7 @@
         <v>456</v>
       </c>
       <c r="B344">
-        <v>124.8</v>
+        <v>946.2</v>
       </c>
     </row>
     <row r="345" spans="1:2">
@@ -18811,7 +18811,7 @@
         <v>457</v>
       </c>
       <c r="B346">
-        <v>124.8</v>
+        <v>946.2</v>
       </c>
     </row>
     <row r="347" spans="1:2">
@@ -18827,7 +18827,7 @@
         <v>458</v>
       </c>
       <c r="B348">
-        <v>124.8</v>
+        <v>946.2</v>
       </c>
     </row>
     <row r="349" spans="1:2">
@@ -18843,7 +18843,7 @@
         <v>459</v>
       </c>
       <c r="B350">
-        <v>124.8</v>
+        <v>946.2</v>
       </c>
     </row>
     <row r="351" spans="1:2">
@@ -18859,7 +18859,7 @@
         <v>460</v>
       </c>
       <c r="B352">
-        <v>124.8</v>
+        <v>946.2</v>
       </c>
     </row>
     <row r="353" spans="1:2">
@@ -18875,7 +18875,7 @@
         <v>461</v>
       </c>
       <c r="B354">
-        <v>124.8</v>
+        <v>946.2</v>
       </c>
     </row>
     <row r="355" spans="1:2">

</xml_diff>